<commit_message>
Scrap post reunión MAR
</commit_message>
<xml_diff>
--- a/notebooks/data/Analytical_Data.xlsx
+++ b/notebooks/data/Analytical_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/495715c1b5296d13/MB_Magister_ y_ otros/DATA_SCIENCE_UDD/6. CAPSTONE/Capstone_git/notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60D61BD8-C24E-1647-A81B-B93C7D3BC144}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0189B167-EA2D-304A-8182-1697DFEE47B5}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16940" xr2:uid="{8FBF2DF0-06EB-D848-B9CF-1FB6A717065A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="177">
   <si>
     <t>per101</t>
   </si>
@@ -483,6 +483,90 @@
   </si>
   <si>
     <t>Variable_per</t>
+  </si>
+  <si>
+    <t>Inmigración</t>
+  </si>
+  <si>
+    <t>DDHH</t>
+  </si>
+  <si>
+    <t>Pueblos originarios</t>
+  </si>
+  <si>
+    <t>Medio ambiente</t>
+  </si>
+  <si>
+    <t>+ Derechos sociales</t>
+  </si>
+  <si>
+    <t>607.3, 608.3</t>
+  </si>
+  <si>
+    <t>Inclusión y Minorías</t>
+  </si>
+  <si>
+    <t>201.2, 503</t>
+  </si>
+  <si>
+    <t>605.1, 605.2</t>
+  </si>
+  <si>
+    <t>Qué tópicos aparecieron en Chile antes que en otros países?</t>
+  </si>
+  <si>
+    <t>503, 705, 606.1</t>
+  </si>
+  <si>
+    <t>Orden, Corrupción, Instituciones debilitadas, Justicia</t>
+  </si>
+  <si>
+    <t>602.2, 607.1</t>
+  </si>
+  <si>
+    <t>Cómo (dónde, cuándo) emergen y evolucionan ciertos tópicos hasta llegar a los programas presidenciales chilenos</t>
+  </si>
+  <si>
+    <t>Cuánto tardó en llegar a Chile con la misma fuerza?</t>
+  </si>
+  <si>
+    <t>PREGUNTAS</t>
+  </si>
+  <si>
+    <t>ENTENDER LAS DINÁMICAS SOCIALES Y POLÍTICAS A NIVEL GLOBAL Y CÓMO LLEGAN A CHILE</t>
+  </si>
+  <si>
+    <t>Hay patrones?</t>
+  </si>
+  <si>
+    <t>Hay países o regiones cuyos discursos influencien los discursos chilenos?</t>
+  </si>
+  <si>
+    <t>Comparación entre Chile y los países de la misma región</t>
+  </si>
+  <si>
+    <t>Tomar chile</t>
+  </si>
+  <si>
+    <t>para cada elección, sumar, promediar, ponderar (lo que defina como razonable y defendible), cada variable 'per'</t>
+  </si>
+  <si>
+    <t>hacer una red de similaridad   y ver si el resultado es coherente copn lo que yo esperaría para chile en esos añois</t>
+  </si>
+  <si>
+    <t>elegir el feature vector para cada tema de interés. Por ej.: inclusión (per1, per2, per4), inmigración (per 2, per7, per8), seguridad (per10, per15)</t>
+  </si>
+  <si>
+    <t>issues en approach inicial:</t>
+  </si>
+  <si>
+    <t>1.hay evenbtos que influencian los programas en ciertos países, que no tienen relación con chile. por ejemplo, una guerra.-</t>
+  </si>
+  <si>
+    <t>2.hay temas muy locaes que infliuencian los programas en chile y no en el extranjero. Ej. La ley Zamudio</t>
+  </si>
+  <si>
+    <t>3. considerar el efecto del cambio de régimen electoral (proporcional a …....)</t>
   </si>
 </sst>
 </file>
@@ -502,12 +586,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -522,8 +612,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,6 +635,539 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>349252</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>86021</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7225AFC2-D095-9FD7-9D45-21610B78FD4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12784669" y="5577417"/>
+          <a:ext cx="5365750" cy="1144354"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1195917</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>929589</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2364B119-B888-2533-9722-8ED1EF1AA826}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12668250" y="6826251"/>
+          <a:ext cx="6062506" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>421018</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAA2CEB-2D74-E8DE-7756-0A4A080CD186}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12784668" y="11070166"/>
+          <a:ext cx="7342517" cy="730250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1248833</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>179917</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>128135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33ADBAD5-C508-1D41-811B-3DB996561B06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12721166" y="15314082"/>
+          <a:ext cx="6212418" cy="1503969"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>180368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDFD293-C874-8243-8383-F71CC19C7D3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12795250" y="19462750"/>
+          <a:ext cx="6921500" cy="2868535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466050</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>31751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36F253CE-78AB-A241-81ED-45D622C8673C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12795250" y="13303250"/>
+          <a:ext cx="5471967" cy="1005418"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>158748</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>656167</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>72983</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DAF8871-324D-6C47-9D78-F010C1E3C4A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12848168" y="14435665"/>
+          <a:ext cx="5609166" cy="517485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>21168</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>793751</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A3E869E-73C8-2346-886E-51DA40993A08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12805835" y="9143999"/>
+          <a:ext cx="6741583" cy="998752"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1301752</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>169334</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>7922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FE1AE62-5222-E046-B2E6-F430E140555F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12774085" y="10191750"/>
+          <a:ext cx="6148916" cy="674672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>21165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>109486</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF780D48-07C2-C44B-AEDA-DC1BEBCB5A5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12784667" y="17113248"/>
+          <a:ext cx="6078486" cy="1555752"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>21165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>10585</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>50950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C5032C-64BA-5344-AA63-82BCB45BA98F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12784668" y="7662332"/>
+          <a:ext cx="5979584" cy="1236285"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1291167</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>328083</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>181271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1299AAC-BF5A-4948-B703-FEC196790BD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12763500" y="11906251"/>
+          <a:ext cx="5365750" cy="1144354"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -858,16 +1487,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4673C131-828D-9D45-9B63-66333BEA4CE5}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1094,7 +1729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -1107,8 +1742,11 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1121,8 +1759,11 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1135,8 +1776,11 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1149,8 +1793,11 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -1164,7 +1811,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -1177,8 +1824,11 @@
       <c r="D22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -1191,8 +1841,11 @@
       <c r="D23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -1205,8 +1858,11 @@
       <c r="D24" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1219,8 +1875,11 @@
       <c r="D25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -1233,8 +1892,11 @@
       <c r="D26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1247,8 +1909,11 @@
       <c r="D27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1261,8 +1926,11 @@
       <c r="D28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="F28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -1276,7 +1944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -1290,7 +1958,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -1303,8 +1971,14 @@
       <c r="D31" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="F31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1318,7 +1992,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -1332,7 +2006,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1346,7 +2020,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -1360,7 +2034,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -1374,7 +2048,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -1388,7 +2062,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -1402,7 +2076,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -1412,11 +2086,11 @@
       <c r="C39" t="s">
         <v>72</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1430,7 +2104,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -1444,7 +2118,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -1458,7 +2132,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -1472,7 +2146,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1486,7 +2160,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -1500,7 +2174,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -1514,7 +2188,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -1528,7 +2202,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -1541,8 +2215,14 @@
       <c r="D48" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -1556,7 +2236,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1570,7 +2250,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>84</v>
       </c>
@@ -1584,7 +2264,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -1598,7 +2278,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -1612,7 +2292,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>112</v>
       </c>
@@ -1626,7 +2306,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -1640,7 +2320,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>112</v>
       </c>
@@ -1654,7 +2334,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -1668,7 +2348,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -1681,8 +2361,14 @@
       <c r="D58" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="F58" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -1696,7 +2382,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -1710,7 +2396,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -1724,7 +2410,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -1738,7 +2424,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>145</v>
       </c>
@@ -1752,7 +2438,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -1766,7 +2452,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>145</v>
       </c>
@@ -1780,7 +2466,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>145</v>
       </c>
@@ -1792,10 +2478,83 @@
       </c>
       <c r="D66" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="F68" t="s">
+        <v>151</v>
+      </c>
+      <c r="G68" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="F78" t="s">
+        <v>152</v>
+      </c>
+      <c r="G78">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="87" spans="6:7">
+      <c r="F87" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G87">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="98" spans="6:7" ht="34">
+      <c r="F98" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="6:6">
+      <c r="F113" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" spans="6:6">
+      <c r="F114" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" spans="6:6">
+      <c r="F115" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" spans="6:6">
+      <c r="F116" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="118" spans="6:6">
+      <c r="F118" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="6:6">
+      <c r="F119" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="120" spans="6:6">
+      <c r="F120" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="121" spans="6:6">
+      <c r="F121" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
df ponderados según Inclusión y Minorías
</commit_message>
<xml_diff>
--- a/notebooks/data/Analytical_Data.xlsx
+++ b/notebooks/data/Analytical_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/495715c1b5296d13/MB_Magister_ y_ otros/DATA_SCIENCE_UDD/6. CAPSTONE/Capstone_git/notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A252CCA9-E870-9742-9806-685E442CF80E}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48730B4A-C7B0-E54E-BE3D-79A3EF90ADA8}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="800" windowWidth="28100" windowHeight="16940" xr2:uid="{8FBF2DF0-06EB-D848-B9CF-1FB6A717065A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="299">
   <si>
     <t>per101</t>
   </si>
@@ -452,9 +452,6 @@
     <t>Privatisation: Positive</t>
   </si>
   <si>
-    <t>per201_1</t>
-  </si>
-  <si>
     <t>Freedom</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>Dominio</t>
   </si>
   <si>
-    <t>Otros</t>
-  </si>
-  <si>
     <t>Detalle_Dominio</t>
   </si>
   <si>
@@ -485,90 +479,6 @@
     <t>Variable_per</t>
   </si>
   <si>
-    <t>Inmigración</t>
-  </si>
-  <si>
-    <t>DDHH</t>
-  </si>
-  <si>
-    <t>Pueblos originarios</t>
-  </si>
-  <si>
-    <t>Medio ambiente</t>
-  </si>
-  <si>
-    <t>+ Derechos sociales</t>
-  </si>
-  <si>
-    <t>607.3, 608.3</t>
-  </si>
-  <si>
-    <t>Inclusión y Minorías</t>
-  </si>
-  <si>
-    <t>201.2, 503</t>
-  </si>
-  <si>
-    <t>605.1, 605.2</t>
-  </si>
-  <si>
-    <t>Qué tópicos aparecieron en Chile antes que en otros países?</t>
-  </si>
-  <si>
-    <t>503, 705, 606.1</t>
-  </si>
-  <si>
-    <t>Orden, Corrupción, Instituciones debilitadas, Justicia</t>
-  </si>
-  <si>
-    <t>602.2, 607.1</t>
-  </si>
-  <si>
-    <t>Cómo (dónde, cuándo) emergen y evolucionan ciertos tópicos hasta llegar a los programas presidenciales chilenos</t>
-  </si>
-  <si>
-    <t>Cuánto tardó en llegar a Chile con la misma fuerza?</t>
-  </si>
-  <si>
-    <t>PREGUNTAS</t>
-  </si>
-  <si>
-    <t>ENTENDER LAS DINÁMICAS SOCIALES Y POLÍTICAS A NIVEL GLOBAL Y CÓMO LLEGAN A CHILE</t>
-  </si>
-  <si>
-    <t>Hay patrones?</t>
-  </si>
-  <si>
-    <t>Hay países o regiones cuyos discursos influencien los discursos chilenos?</t>
-  </si>
-  <si>
-    <t>Comparación entre Chile y los países de la misma región</t>
-  </si>
-  <si>
-    <t>Tomar chile</t>
-  </si>
-  <si>
-    <t>para cada elección, sumar, promediar, ponderar (lo que defina como razonable y defendible), cada variable 'per'</t>
-  </si>
-  <si>
-    <t>hacer una red de similaridad   y ver si el resultado es coherente copn lo que yo esperaría para chile en esos añois</t>
-  </si>
-  <si>
-    <t>elegir el feature vector para cada tema de interés. Por ej.: inclusión (per1, per2, per4), inmigración (per 2, per7, per8), seguridad (per10, per15)</t>
-  </si>
-  <si>
-    <t>issues en approach inicial:</t>
-  </si>
-  <si>
-    <t>1.hay evenbtos que influencian los programas en ciertos países, que no tienen relación con chile. por ejemplo, una guerra.-</t>
-  </si>
-  <si>
-    <t>2.hay temas muy locaes que infliuencian los programas en chile y no en el extranjero. Ej. La ley Zamudio</t>
-  </si>
-  <si>
-    <t>3. considerar el efecto del cambio de régimen electoral (proporcional a …....)</t>
-  </si>
-  <si>
     <t>per1011</t>
   </si>
   <si>
@@ -837,13 +747,199 @@
   </si>
   <si>
     <t>Minorities Inland: Positive</t>
+  </si>
+  <si>
+    <t>per7052</t>
+  </si>
+  <si>
+    <t>per7061</t>
+  </si>
+  <si>
+    <t>per7062</t>
+  </si>
+  <si>
+    <t>Minorities Abroad: Positive</t>
+  </si>
+  <si>
+    <t>War Participants: Positive</t>
+  </si>
+  <si>
+    <t>Refugees: Positive</t>
+  </si>
+  <si>
+    <t>per103_1</t>
+  </si>
+  <si>
+    <t>per703_2</t>
+  </si>
+  <si>
+    <t>Anti-Imperialism: State Centred Anti-Imperialism</t>
+  </si>
+  <si>
+    <t>per103-2</t>
+  </si>
+  <si>
+    <t>Anti-Imperialism: Foreign Financial Influence</t>
+  </si>
+  <si>
+    <t>per201-1</t>
+  </si>
+  <si>
+    <t>per202_2</t>
+  </si>
+  <si>
+    <t>Democracy General: Negative</t>
+  </si>
+  <si>
+    <t>per202_3</t>
+  </si>
+  <si>
+    <t>Representative Democracy: Positive</t>
+  </si>
+  <si>
+    <t>per202_4</t>
+  </si>
+  <si>
+    <t>Direct Democracy: Positive</t>
+  </si>
+  <si>
+    <t>per305_1</t>
+  </si>
+  <si>
+    <t>Political Authority: Party Competence</t>
+  </si>
+  <si>
+    <t>per305_2</t>
+  </si>
+  <si>
+    <t>Political Authority: Personal Competence</t>
+  </si>
+  <si>
+    <t>per305_3</t>
+  </si>
+  <si>
+    <t>Political Authority: Strong government</t>
+  </si>
+  <si>
+    <t>per305_4</t>
+  </si>
+  <si>
+    <t>Transition: Pre-Democratic Elites: Positive</t>
+  </si>
+  <si>
+    <t>per305_5</t>
+  </si>
+  <si>
+    <t>Transition: Pre-Democratic Elites: Negative</t>
+  </si>
+  <si>
+    <t>per305_6</t>
+  </si>
+  <si>
+    <t>Transition: Rehabilitation and Compensation</t>
+  </si>
+  <si>
+    <t>per416_1</t>
+  </si>
+  <si>
+    <t>per416_2</t>
+  </si>
+  <si>
+    <t>Sustainability: Positive</t>
+  </si>
+  <si>
+    <t>per601_1</t>
+  </si>
+  <si>
+    <t>National Way of Life General: Positive</t>
+  </si>
+  <si>
+    <t>per601_2</t>
+  </si>
+  <si>
+    <t>National Way of Life: Immigration: Negative</t>
+  </si>
+  <si>
+    <t>per602_1</t>
+  </si>
+  <si>
+    <t>National Way of Life General: Negative</t>
+  </si>
+  <si>
+    <t>per602_2</t>
+  </si>
+  <si>
+    <t>National Way of Life: Immigration: Positive</t>
+  </si>
+  <si>
+    <t>per605_1</t>
+  </si>
+  <si>
+    <t>per605_2</t>
+  </si>
+  <si>
+    <t>Law and Order: Negative</t>
+  </si>
+  <si>
+    <t>per606_1</t>
+  </si>
+  <si>
+    <t>Civic Mindedness General: Positive</t>
+  </si>
+  <si>
+    <t>per606_2</t>
+  </si>
+  <si>
+    <t>Civic Mindedness: Bottom-Up Activism</t>
+  </si>
+  <si>
+    <t>per607_1</t>
+  </si>
+  <si>
+    <t>Multiculturalism General: Positive</t>
+  </si>
+  <si>
+    <t>per607_2</t>
+  </si>
+  <si>
+    <t>Multiculturalism: Immigrants Diversity</t>
+  </si>
+  <si>
+    <t>per607_3</t>
+  </si>
+  <si>
+    <t>Multiculturalism: Indigenous rights: Positive</t>
+  </si>
+  <si>
+    <t>per608_1</t>
+  </si>
+  <si>
+    <t>Multiculturalism General: Negative</t>
+  </si>
+  <si>
+    <t>per608_2</t>
+  </si>
+  <si>
+    <t>Multiculturalism: Immigrants Assimilation</t>
+  </si>
+  <si>
+    <t>per608_3</t>
+  </si>
+  <si>
+    <t>Multiculturalism: Indigenous rights: Negative</t>
+  </si>
+  <si>
+    <t>per703_1</t>
+  </si>
+  <si>
+    <t>Agriculture and Farmers: Negative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -855,19 +951,19 @@
       <name val="ArialMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -882,13 +978,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,539 +996,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>148167</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>349252</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>86021</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7225AFC2-D095-9FD7-9D45-21610B78FD4D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12784669" y="5577417"/>
-          <a:ext cx="5365750" cy="1144354"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1195917</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>929589</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>148167</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2364B119-B888-2533-9722-8ED1EF1AA826}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12668250" y="6826251"/>
-          <a:ext cx="6062506" cy="762000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>10583</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>421018</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>137583</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAA2CEB-2D74-E8DE-7756-0A4A080CD186}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12784668" y="11070166"/>
-          <a:ext cx="7342517" cy="730250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1248833</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>179917</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>128135</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33ADBAD5-C508-1D41-811B-3DB996561B06}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12721166" y="15314082"/>
-          <a:ext cx="6212418" cy="1503969"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>180368</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDFD293-C874-8243-8383-F71CC19C7D3C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12795250" y="19462750"/>
-          <a:ext cx="6921500" cy="2868535"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>466050</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>31751</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36F253CE-78AB-A241-81ED-45D622C8673C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12795250" y="13303250"/>
-          <a:ext cx="5471967" cy="1005418"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>63501</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>158748</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>656167</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>72983</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DAF8871-324D-6C47-9D78-F010C1E3C4A1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12848168" y="14435665"/>
-          <a:ext cx="5609166" cy="517485"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>21168</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>793751</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>88584</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A3E869E-73C8-2346-886E-51DA40993A08}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12805835" y="9143999"/>
-          <a:ext cx="6741583" cy="998752"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1301752</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>137583</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>169334</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>7922</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FE1AE62-5222-E046-B2E6-F430E140555F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12774085" y="10191750"/>
-          <a:ext cx="6148916" cy="674672"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>21165</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>109486</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF780D48-07C2-C44B-AEDA-DC1BEBCB5A5A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12784667" y="17113248"/>
-          <a:ext cx="6078486" cy="1555752"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>21165</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>10585</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>50950</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C5032C-64BA-5344-AA63-82BCB45BA98F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12784668" y="7662332"/>
-          <a:ext cx="5979584" cy="1236285"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1291167</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>42334</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>328083</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>181271</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1299AAC-BF5A-4948-B703-FEC196790BD4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12763500" y="11906251"/>
-          <a:ext cx="5365750" cy="1144354"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1756,36 +1315,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4673C131-828D-9D45-9B63-66333BEA4CE5}">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C109" sqref="C109"/>
+      <selection pane="bottomRight" activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
         <v>144</v>
-      </c>
-      <c r="B1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1998,7 +1554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -2011,11 +1567,8 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -2028,11 +1581,8 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2045,11 +1595,8 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2062,11 +1609,8 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="F20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -2080,7 +1624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -2093,11 +1637,8 @@
       <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -2110,11 +1651,8 @@
       <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="F23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -2127,11 +1665,8 @@
       <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="F24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -2144,11 +1679,8 @@
       <c r="D25" t="s">
         <v>58</v>
       </c>
-      <c r="F25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2161,11 +1693,8 @@
       <c r="D26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -2178,11 +1707,8 @@
       <c r="D27" t="s">
         <v>60</v>
       </c>
-      <c r="F27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2195,11 +1721,8 @@
       <c r="D28" t="s">
         <v>61</v>
       </c>
-      <c r="F28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2213,7 +1736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -2227,7 +1750,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2240,14 +1763,8 @@
       <c r="D31" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -2261,7 +1778,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -2275,7 +1792,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2289,7 +1806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -2303,7 +1820,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -2317,7 +1834,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -2331,7 +1848,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -2345,7 +1862,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2359,7 +1876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -2373,7 +1890,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -2387,7 +1904,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -2401,7 +1918,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2415,7 +1932,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2429,7 +1946,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2443,7 +1960,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -2457,7 +1974,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2471,7 +1988,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -2484,14 +2001,8 @@
       <c r="D48" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -2505,7 +2016,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -2519,7 +2030,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>84</v>
       </c>
@@ -2533,7 +2044,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -2547,7 +2058,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -2561,7 +2072,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>112</v>
       </c>
@@ -2575,7 +2086,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -2589,7 +2100,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>112</v>
       </c>
@@ -2603,7 +2114,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2617,249 +2128,405 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
       <c r="C58" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" t="s">
+        <v>151</v>
+      </c>
+      <c r="D60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" t="s">
+        <v>154</v>
+      </c>
+      <c r="D62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D64" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" t="s">
+        <v>159</v>
+      </c>
+      <c r="D67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" t="s">
         <v>177</v>
       </c>
-      <c r="D58" t="s">
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" t="s">
         <v>178</v>
       </c>
-      <c r="F58" t="s">
-        <v>150</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="C59" t="s">
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" t="s">
         <v>179</v>
       </c>
-      <c r="D59" t="s">
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" t="s">
+        <v>163</v>
+      </c>
+      <c r="D71" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="C60" t="s">
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" t="s">
         <v>181</v>
       </c>
-      <c r="D60" t="s">
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="C61" t="s">
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" t="s">
+        <v>166</v>
+      </c>
+      <c r="D74" t="s">
         <v>183</v>
       </c>
-      <c r="D61" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="C62" t="s">
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" t="s">
+        <v>167</v>
+      </c>
+      <c r="D75" t="s">
         <v>184</v>
       </c>
-      <c r="D62" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="C63" t="s">
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" t="s">
         <v>185</v>
       </c>
-      <c r="D63" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="C64" t="s">
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" t="s">
         <v>186</v>
       </c>
-      <c r="D64" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="65" spans="3:7">
-      <c r="C65" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="66" spans="3:7">
-      <c r="C66" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="3:7">
-      <c r="C67" t="s">
-        <v>189</v>
-      </c>
-      <c r="D67" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="68" spans="3:7">
-      <c r="C68" t="s">
-        <v>190</v>
-      </c>
-      <c r="D68" t="s">
-        <v>207</v>
-      </c>
-      <c r="F68" t="s">
-        <v>151</v>
-      </c>
-      <c r="G68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="3:7">
-      <c r="C69" t="s">
-        <v>191</v>
-      </c>
-      <c r="D69" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="70" spans="3:7">
-      <c r="C70" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="71" spans="3:7">
-      <c r="C71" t="s">
-        <v>193</v>
-      </c>
-      <c r="D71" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="72" spans="3:7">
-      <c r="C72" t="s">
-        <v>194</v>
-      </c>
-      <c r="D72" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="73" spans="3:7">
-      <c r="C73" t="s">
-        <v>195</v>
-      </c>
-      <c r="D73" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="74" spans="3:7">
-      <c r="C74" t="s">
-        <v>196</v>
-      </c>
-      <c r="D74" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="75" spans="3:7">
-      <c r="C75" t="s">
-        <v>197</v>
-      </c>
-      <c r="D75" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="76" spans="3:7">
-      <c r="C76" t="s">
-        <v>198</v>
-      </c>
-      <c r="D76" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="77" spans="3:7">
-      <c r="C77" t="s">
-        <v>199</v>
-      </c>
-      <c r="D77" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="78" spans="3:7">
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" t="s">
+        <v>96</v>
+      </c>
       <c r="C78" t="s">
         <v>126</v>
       </c>
       <c r="D78" t="s">
         <v>127</v>
       </c>
-      <c r="F78" t="s">
-        <v>152</v>
-      </c>
-      <c r="G78">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="79" spans="3:7">
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" t="s">
+        <v>96</v>
+      </c>
       <c r="C79" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="D79" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="3:7">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" t="s">
+        <v>98</v>
+      </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="81" spans="3:7">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" t="s">
+        <v>98</v>
+      </c>
       <c r="C81" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="D81" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="82" spans="3:7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" t="s">
+        <v>98</v>
+      </c>
       <c r="C82" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="D82" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="83" spans="3:7">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" t="s">
+        <v>98</v>
+      </c>
       <c r="C83" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="D83" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" t="s">
+        <v>98</v>
+      </c>
       <c r="C84" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="D84" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="85" spans="3:7">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>99</v>
+      </c>
+      <c r="B85" t="s">
+        <v>98</v>
+      </c>
       <c r="C85" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="D85" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="86" spans="3:7">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>100</v>
+      </c>
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
       <c r="C86" t="s">
         <v>136</v>
       </c>
@@ -2867,53 +2534,83 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="3:7">
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" t="s">
+        <v>101</v>
+      </c>
       <c r="C87" t="s">
         <v>129</v>
       </c>
       <c r="D87" t="s">
         <v>128</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G87">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="88" spans="3:7">
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="D88" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="89" spans="3:7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="D89" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="90" spans="3:7">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" t="s">
+        <v>101</v>
+      </c>
       <c r="C90" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="D90" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="91" spans="3:7">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
       <c r="C91" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="D91" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="92" spans="3:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" t="s">
+        <v>101</v>
+      </c>
       <c r="C92" t="s">
         <v>131</v>
       </c>
@@ -2921,7 +2618,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="3:7">
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" t="s">
+        <v>101</v>
+      </c>
       <c r="C93" t="s">
         <v>133</v>
       </c>
@@ -2929,53 +2632,83 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="3:7">
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" t="s">
+        <v>101</v>
+      </c>
       <c r="C94" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="D94" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="95" spans="3:7">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" t="s">
+        <v>101</v>
+      </c>
       <c r="C95" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="D95" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="96" spans="3:7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" t="s">
+        <v>102</v>
+      </c>
       <c r="C96" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D96" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="97" spans="3:7">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" t="s">
+        <v>102</v>
+      </c>
       <c r="C97" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="D97" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="98" spans="3:7" ht="34">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98" t="s">
+        <v>102</v>
+      </c>
       <c r="C98" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D98" t="s">
-        <v>256</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="3:7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" t="s">
+        <v>102</v>
+      </c>
       <c r="C99" t="s">
         <v>135</v>
       </c>
@@ -2983,245 +2716,668 @@
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="3:7">
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" t="s">
+        <v>85</v>
+      </c>
       <c r="C100" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="D100" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>84</v>
+      </c>
+      <c r="B101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>84</v>
+      </c>
+      <c r="B102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C102" t="s">
+        <v>216</v>
+      </c>
+      <c r="D102" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>84</v>
+      </c>
+      <c r="B103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" t="s">
+        <v>217</v>
+      </c>
+      <c r="D103" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B104" t="s">
+        <v>85</v>
+      </c>
+      <c r="C104" t="s">
+        <v>218</v>
+      </c>
+      <c r="D104" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>84</v>
+      </c>
+      <c r="B105" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" t="s">
+        <v>219</v>
+      </c>
+      <c r="D105" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>84</v>
+      </c>
+      <c r="B106" t="s">
+        <v>85</v>
+      </c>
+      <c r="C106" t="s">
+        <v>220</v>
+      </c>
+      <c r="D106" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107" t="s">
+        <v>234</v>
+      </c>
+      <c r="D107" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" t="s">
+        <v>221</v>
+      </c>
+      <c r="D108" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" t="s">
+        <v>237</v>
+      </c>
+      <c r="D109" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="s">
+        <v>113</v>
+      </c>
+      <c r="C110" t="s">
+        <v>238</v>
+      </c>
+      <c r="D110" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" t="s">
+        <v>239</v>
+      </c>
+      <c r="D111" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>94</v>
+      </c>
+      <c r="B112" t="s">
+        <v>95</v>
+      </c>
+      <c r="C112" t="s">
+        <v>243</v>
+      </c>
+      <c r="D112" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>94</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>97</v>
+      </c>
+      <c r="B114" t="s">
+        <v>96</v>
+      </c>
+      <c r="C114" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115" t="s">
+        <v>96</v>
+      </c>
+      <c r="C115" t="s">
+        <v>140</v>
+      </c>
+      <c r="D115" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>97</v>
+      </c>
+      <c r="B116" t="s">
+        <v>96</v>
+      </c>
+      <c r="C116" t="s">
+        <v>142</v>
+      </c>
+      <c r="D116" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>97</v>
+      </c>
+      <c r="B117" t="s">
+        <v>96</v>
+      </c>
+      <c r="C117" t="s">
+        <v>249</v>
+      </c>
+      <c r="D117" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>97</v>
+      </c>
+      <c r="B118" t="s">
+        <v>96</v>
+      </c>
+      <c r="C118" t="s">
+        <v>251</v>
+      </c>
+      <c r="D118" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" t="s">
+        <v>96</v>
+      </c>
+      <c r="C119" t="s">
+        <v>253</v>
+      </c>
+      <c r="D119" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>99</v>
+      </c>
+      <c r="B120" t="s">
+        <v>98</v>
+      </c>
+      <c r="C120" t="s">
+        <v>255</v>
+      </c>
+      <c r="D120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" t="s">
+        <v>98</v>
+      </c>
+      <c r="C121" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="101" spans="3:7">
-      <c r="C101" t="s">
-        <v>245</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="D121" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="102" spans="3:7">
-      <c r="C102" t="s">
-        <v>246</v>
-      </c>
-      <c r="D102" t="s">
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>99</v>
+      </c>
+      <c r="B122" t="s">
+        <v>98</v>
+      </c>
+      <c r="C122" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="103" spans="3:7">
-      <c r="C103" t="s">
-        <v>247</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="D122" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="3:7">
-      <c r="C104" t="s">
-        <v>248</v>
-      </c>
-      <c r="D104" t="s">
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>99</v>
+      </c>
+      <c r="B123" t="s">
+        <v>98</v>
+      </c>
+      <c r="C123" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="105" spans="3:7">
-      <c r="C105" t="s">
-        <v>249</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="D123" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="3:7">
-      <c r="C106" t="s">
-        <v>250</v>
-      </c>
-      <c r="D106" t="s">
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>99</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+      <c r="C124" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="107" spans="3:7">
-      <c r="C107" t="s">
+      <c r="D124" t="s">
         <v>264</v>
       </c>
-      <c r="D107" t="s">
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>99</v>
+      </c>
+      <c r="B125" t="s">
+        <v>98</v>
+      </c>
+      <c r="C125" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="108" spans="3:7">
-      <c r="C108" t="s">
-        <v>251</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="D125" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
-      <c r="F113" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="F114" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="F115" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="F116" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="F118" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="F119" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="F120" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" t="s">
-        <v>145</v>
-      </c>
-      <c r="B121" t="s">
-        <v>145</v>
-      </c>
-      <c r="C121" t="s">
-        <v>126</v>
-      </c>
-      <c r="D121" t="s">
-        <v>127</v>
-      </c>
-      <c r="F121" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" t="s">
-        <v>145</v>
-      </c>
-      <c r="B122" t="s">
-        <v>145</v>
-      </c>
-      <c r="C122" t="s">
-        <v>136</v>
-      </c>
-      <c r="D122" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" t="s">
-        <v>145</v>
-      </c>
-      <c r="B123" t="s">
-        <v>145</v>
-      </c>
-      <c r="C123" t="s">
-        <v>129</v>
-      </c>
-      <c r="D123" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" t="s">
-        <v>145</v>
-      </c>
-      <c r="B124" t="s">
-        <v>145</v>
-      </c>
-      <c r="C124" t="s">
-        <v>131</v>
-      </c>
-      <c r="D124" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" t="s">
-        <v>145</v>
-      </c>
-      <c r="B125" t="s">
-        <v>145</v>
-      </c>
-      <c r="C125" t="s">
-        <v>133</v>
-      </c>
-      <c r="D125" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="B126" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>135</v>
+        <v>267</v>
       </c>
       <c r="D126" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="B127" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="C127" t="s">
-        <v>138</v>
+        <v>268</v>
       </c>
       <c r="D127" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C128" t="s">
-        <v>141</v>
+        <v>270</v>
       </c>
       <c r="D128" t="s">
-        <v>140</v>
+        <v>271</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="B129" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C129" t="s">
-        <v>143</v>
+        <v>272</v>
       </c>
       <c r="D129" t="s">
-        <v>142</v>
-      </c>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>84</v>
+      </c>
+      <c r="B130" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" t="s">
+        <v>274</v>
+      </c>
+      <c r="D130" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>84</v>
+      </c>
+      <c r="B131" t="s">
+        <v>85</v>
+      </c>
+      <c r="C131" t="s">
+        <v>276</v>
+      </c>
+      <c r="D131" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>84</v>
+      </c>
+      <c r="B132" t="s">
+        <v>85</v>
+      </c>
+      <c r="C132" t="s">
+        <v>278</v>
+      </c>
+      <c r="D132" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>84</v>
+      </c>
+      <c r="B133" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133" t="s">
+        <v>279</v>
+      </c>
+      <c r="D133" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>84</v>
+      </c>
+      <c r="B134" t="s">
+        <v>85</v>
+      </c>
+      <c r="C134" t="s">
+        <v>281</v>
+      </c>
+      <c r="D134" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>84</v>
+      </c>
+      <c r="B135" t="s">
+        <v>85</v>
+      </c>
+      <c r="C135" t="s">
+        <v>283</v>
+      </c>
+      <c r="D135" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>84</v>
+      </c>
+      <c r="B136" t="s">
+        <v>85</v>
+      </c>
+      <c r="C136" t="s">
+        <v>285</v>
+      </c>
+      <c r="D136" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>84</v>
+      </c>
+      <c r="B137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C137" t="s">
+        <v>287</v>
+      </c>
+      <c r="D137" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>84</v>
+      </c>
+      <c r="B138" t="s">
+        <v>85</v>
+      </c>
+      <c r="C138" t="s">
+        <v>289</v>
+      </c>
+      <c r="D138" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>84</v>
+      </c>
+      <c r="B139" t="s">
+        <v>85</v>
+      </c>
+      <c r="C139" t="s">
+        <v>291</v>
+      </c>
+      <c r="D139" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>84</v>
+      </c>
+      <c r="B140" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" t="s">
+        <v>293</v>
+      </c>
+      <c r="D140" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>84</v>
+      </c>
+      <c r="B141" t="s">
+        <v>85</v>
+      </c>
+      <c r="C141" t="s">
+        <v>295</v>
+      </c>
+      <c r="D141" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>112</v>
+      </c>
+      <c r="B142" t="s">
+        <v>113</v>
+      </c>
+      <c r="C142" t="s">
+        <v>297</v>
+      </c>
+      <c r="D142" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>112</v>
+      </c>
+      <c r="B143" t="s">
+        <v>113</v>
+      </c>
+      <c r="C143" t="s">
+        <v>244</v>
+      </c>
+      <c r="D143" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="3:4">
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+    </row>
+    <row r="146" spans="3:4">
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+    </row>
+    <row r="147" spans="3:4">
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+    </row>
+    <row r="148" spans="3:4">
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+    </row>
+    <row r="149" spans="3:4">
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+    </row>
+    <row r="150" spans="3:4">
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+    </row>
+    <row r="151" spans="3:4">
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+    </row>
+    <row r="152" spans="3:4">
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="3:4">
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="3:4">
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Análisis Chile, inclusión y minorías, Piñera corregido
</commit_message>
<xml_diff>
--- a/notebooks/data/Analytical_Data.xlsx
+++ b/notebooks/data/Analytical_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/495715c1b5296d13/MB_Magister_ y_ otros/DATA_SCIENCE_UDD/6. CAPSTONE/Capstone_git/notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48730B4A-C7B0-E54E-BE3D-79A3EF90ADA8}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{564137AA-6774-6F4B-A3C5-191B3CF17894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE438BA1-BD4A-8C41-8E5F-9A610F5A8D68}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="800" windowWidth="28100" windowHeight="16940" xr2:uid="{8FBF2DF0-06EB-D848-B9CF-1FB6A717065A}"/>
   </bookViews>
@@ -776,15 +776,9 @@
     <t>Anti-Imperialism: State Centred Anti-Imperialism</t>
   </si>
   <si>
-    <t>per103-2</t>
-  </si>
-  <si>
     <t>Anti-Imperialism: Foreign Financial Influence</t>
   </si>
   <si>
-    <t>per201-1</t>
-  </si>
-  <si>
     <t>per202_2</t>
   </si>
   <si>
@@ -933,6 +927,12 @@
   </si>
   <si>
     <t>Agriculture and Farmers: Negative</t>
+  </si>
+  <si>
+    <t>per103_2</t>
+  </si>
+  <si>
+    <t>per201_1</t>
   </si>
 </sst>
 </file>
@@ -1318,10 +1318,10 @@
   <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B162" sqref="B162"/>
+      <selection pane="bottomRight" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2906,10 +2906,10 @@
         <v>95</v>
       </c>
       <c r="C113" t="s">
+        <v>297</v>
+      </c>
+      <c r="D113" t="s">
         <v>246</v>
-      </c>
-      <c r="D113" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2920,7 +2920,7 @@
         <v>96</v>
       </c>
       <c r="C114" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
       <c r="D114" t="s">
         <v>138</v>
@@ -2962,10 +2962,10 @@
         <v>96</v>
       </c>
       <c r="C117" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D117" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2976,10 +2976,10 @@
         <v>96</v>
       </c>
       <c r="C118" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D118" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2990,10 +2990,10 @@
         <v>96</v>
       </c>
       <c r="C119" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D119" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3004,10 +3004,10 @@
         <v>98</v>
       </c>
       <c r="C120" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D120" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3018,10 +3018,10 @@
         <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D121" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3032,10 +3032,10 @@
         <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D122" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3046,10 +3046,10 @@
         <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D123" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3060,10 +3060,10 @@
         <v>98</v>
       </c>
       <c r="C124" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D124" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3074,10 +3074,10 @@
         <v>98</v>
       </c>
       <c r="C125" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D125" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3088,7 +3088,7 @@
         <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D126" t="s">
         <v>69</v>
@@ -3102,10 +3102,10 @@
         <v>101</v>
       </c>
       <c r="C127" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D127" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3116,10 +3116,10 @@
         <v>85</v>
       </c>
       <c r="C128" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D128" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3130,10 +3130,10 @@
         <v>85</v>
       </c>
       <c r="C129" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D129" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3144,10 +3144,10 @@
         <v>85</v>
       </c>
       <c r="C130" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D130" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3158,10 +3158,10 @@
         <v>85</v>
       </c>
       <c r="C131" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D131" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3172,7 +3172,7 @@
         <v>85</v>
       </c>
       <c r="C132" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D132" t="s">
         <v>108</v>
@@ -3186,10 +3186,10 @@
         <v>85</v>
       </c>
       <c r="C133" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D133" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3200,10 +3200,10 @@
         <v>85</v>
       </c>
       <c r="C134" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D134" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3214,10 +3214,10 @@
         <v>85</v>
       </c>
       <c r="C135" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D135" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3228,10 +3228,10 @@
         <v>85</v>
       </c>
       <c r="C136" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D136" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3242,10 +3242,10 @@
         <v>85</v>
       </c>
       <c r="C137" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D137" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3256,10 +3256,10 @@
         <v>85</v>
       </c>
       <c r="C138" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D138" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3270,10 +3270,10 @@
         <v>85</v>
       </c>
       <c r="C139" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D139" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3284,10 +3284,10 @@
         <v>85</v>
       </c>
       <c r="C140" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D140" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3298,10 +3298,10 @@
         <v>85</v>
       </c>
       <c r="C141" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D141" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3312,7 +3312,7 @@
         <v>113</v>
       </c>
       <c r="C142" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D142" t="s">
         <v>122</v>
@@ -3329,7 +3329,7 @@
         <v>244</v>
       </c>
       <c r="D143" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="144" spans="1:4">

</xml_diff>